<commit_message>
Distribució i llistat dispositius domòtics
</commit_message>
<xml_diff>
--- a/Material_Projecte_HAss_CM.xlsx
+++ b/Material_Projecte_HAss_CM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_DISCO_D\_Imprimir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_DISCO_D\Lluis\ClubMaker\2022-2023 Ferran Fàbregas\Home Assistant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D183F8-6CE9-4629-BC8B-767E0DCBB152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98529988-6033-45E3-8677-96D9B764EA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{90EF32AE-CA61-4A13-A861-A0582E42A800}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="76">
   <si>
     <t>MATERIAL PROJECTE HOME ASSISTANT CLUB MAKER</t>
   </si>
@@ -351,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -380,6 +380,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -882,13 +887,13 @@
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>41</v>
+        <v>66</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10">
@@ -902,15 +907,17 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>65</v>
+      <c r="A11" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>41</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11">
@@ -924,14 +931,14 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="7"/>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="5"/>
+      <c r="B12" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>41</v>
       </c>
       <c r="E12" s="14"/>
@@ -946,16 +953,14 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E13" s="14"/>
@@ -977,9 +982,7 @@
       <c r="C14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>65</v>
-      </c>
+      <c r="D14" s="5"/>
       <c r="E14" s="13" t="s">
         <v>69</v>
       </c>
@@ -1124,6 +1127,10 @@
         <v>42</v>
       </c>
       <c r="E21" s="10"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="7"/>

</xml_diff>